<commit_message>
Actualizacion del repo v1
</commit_message>
<xml_diff>
--- a/dataR2.xlsx
+++ b/dataR2.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faltamira\tareaPCA\PCA-Breast-Cancer\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C98166D-CCCD-4CCC-949D-46CB50F5FF7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="645" windowWidth="22695" windowHeight="7365"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -55,7 +61,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -97,14 +103,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -142,7 +151,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -214,7 +223,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -387,16 +396,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -428,7 +437,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>48</v>
       </c>
@@ -460,7 +469,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>83</v>
       </c>
@@ -492,7 +501,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>82</v>
       </c>
@@ -524,7 +533,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>68</v>
       </c>
@@ -556,7 +565,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>86</v>
       </c>
@@ -588,7 +597,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>49</v>
       </c>
@@ -620,7 +629,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>89</v>
       </c>
@@ -652,7 +661,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>76</v>
       </c>
@@ -684,7 +693,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>73</v>
       </c>
@@ -716,7 +725,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>75</v>
       </c>
@@ -748,7 +757,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>34</v>
       </c>
@@ -780,7 +789,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>29</v>
       </c>
@@ -812,7 +821,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>25</v>
       </c>
@@ -844,7 +853,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>24</v>
       </c>
@@ -876,7 +885,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>38</v>
       </c>
@@ -908,7 +917,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>44</v>
       </c>
@@ -940,7 +949,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>47</v>
       </c>
@@ -972,7 +981,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>61</v>
       </c>
@@ -1004,7 +1013,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>64</v>
       </c>
@@ -1036,7 +1045,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>32</v>
       </c>
@@ -1068,7 +1077,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>36</v>
       </c>
@@ -1100,7 +1109,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>34</v>
       </c>
@@ -1132,7 +1141,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>29</v>
       </c>
@@ -1164,7 +1173,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>35</v>
       </c>
@@ -1196,7 +1205,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>54</v>
       </c>
@@ -1228,7 +1237,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>45</v>
       </c>
@@ -1260,7 +1269,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>50</v>
       </c>
@@ -1292,7 +1301,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>66</v>
       </c>
@@ -1324,7 +1333,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>35</v>
       </c>
@@ -1356,7 +1365,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>36</v>
       </c>
@@ -1388,7 +1397,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>66</v>
       </c>
@@ -1420,7 +1429,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>53</v>
       </c>
@@ -1452,7 +1461,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>28</v>
       </c>
@@ -1484,7 +1493,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>43</v>
       </c>
@@ -1516,7 +1525,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>51</v>
       </c>
@@ -1548,7 +1557,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>67</v>
       </c>
@@ -1580,7 +1589,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>66</v>
       </c>
@@ -1612,7 +1621,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>69</v>
       </c>
@@ -1644,7 +1653,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>60</v>
       </c>
@@ -1676,7 +1685,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>77</v>
       </c>
@@ -1708,7 +1717,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>76</v>
       </c>
@@ -1740,7 +1749,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>76</v>
       </c>
@@ -1772,7 +1781,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>75</v>
       </c>
@@ -1804,7 +1813,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>69</v>
       </c>
@@ -1836,7 +1845,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>71</v>
       </c>
@@ -1868,7 +1877,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>66</v>
       </c>
@@ -1900,7 +1909,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>75</v>
       </c>
@@ -1932,7 +1941,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>78</v>
       </c>
@@ -1964,7 +1973,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>69</v>
       </c>
@@ -1996,7 +2005,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>85</v>
       </c>
@@ -2028,7 +2037,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>76</v>
       </c>
@@ -2060,7 +2069,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>77</v>
       </c>
@@ -2092,7 +2101,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>45</v>
       </c>
@@ -2124,7 +2133,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>45</v>
       </c>
@@ -2156,7 +2165,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>49</v>
       </c>
@@ -2188,7 +2197,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>34</v>
       </c>
@@ -2220,7 +2229,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>42</v>
       </c>
@@ -2252,7 +2261,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>68</v>
       </c>
@@ -2284,7 +2293,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>51</v>
       </c>
@@ -2316,7 +2325,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>62</v>
       </c>
@@ -2348,7 +2357,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>38</v>
       </c>
@@ -2380,7 +2389,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>69</v>
       </c>
@@ -2412,7 +2421,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>49</v>
       </c>
@@ -2444,7 +2453,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>51</v>
       </c>
@@ -2476,7 +2485,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>59</v>
       </c>
@@ -2508,7 +2517,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>45</v>
       </c>
@@ -2540,7 +2549,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>54</v>
       </c>
@@ -2572,7 +2581,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>64</v>
       </c>
@@ -2604,7 +2613,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>46</v>
       </c>
@@ -2636,7 +2645,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>44</v>
       </c>
@@ -2668,7 +2677,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>45</v>
       </c>
@@ -2700,7 +2709,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>44</v>
       </c>
@@ -2732,7 +2741,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>51</v>
       </c>
@@ -2764,7 +2773,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>72</v>
       </c>
@@ -2796,7 +2805,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>46</v>
       </c>
@@ -2828,7 +2837,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>43</v>
       </c>
@@ -2860,7 +2869,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>55</v>
       </c>
@@ -2892,7 +2901,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>43</v>
       </c>
@@ -2924,7 +2933,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>86</v>
       </c>
@@ -2956,7 +2965,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>41</v>
       </c>
@@ -2988,7 +2997,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>59</v>
       </c>
@@ -3020,7 +3029,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>81</v>
       </c>
@@ -3052,7 +3061,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>48</v>
       </c>
@@ -3084,7 +3093,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>71</v>
       </c>
@@ -3116,7 +3125,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>42</v>
       </c>
@@ -3148,7 +3157,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>65</v>
       </c>
@@ -3180,7 +3189,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>48</v>
       </c>
@@ -3212,7 +3221,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>85</v>
       </c>
@@ -3244,7 +3253,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>48</v>
       </c>
@@ -3276,7 +3285,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>58</v>
       </c>
@@ -3308,7 +3317,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>40</v>
       </c>
@@ -3340,7 +3349,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>82</v>
       </c>
@@ -3372,7 +3381,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>52</v>
       </c>
@@ -3404,7 +3413,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>49</v>
       </c>
@@ -3436,7 +3445,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>60</v>
       </c>
@@ -3468,7 +3477,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>49</v>
       </c>
@@ -3500,7 +3509,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>44</v>
       </c>
@@ -3532,7 +3541,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>40</v>
       </c>
@@ -3564,7 +3573,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>71</v>
       </c>
@@ -3596,7 +3605,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>69</v>
       </c>
@@ -3628,7 +3637,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>74</v>
       </c>
@@ -3660,7 +3669,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>66</v>
       </c>
@@ -3692,7 +3701,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>65</v>
       </c>
@@ -3724,7 +3733,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>72</v>
       </c>
@@ -3756,7 +3765,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>57</v>
       </c>
@@ -3788,7 +3797,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>73</v>
       </c>
@@ -3820,7 +3829,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>45</v>
       </c>
@@ -3852,7 +3861,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>46</v>
       </c>
@@ -3884,7 +3893,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>68</v>
       </c>
@@ -3916,7 +3925,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>75</v>
       </c>
@@ -3948,7 +3957,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>54</v>
       </c>
@@ -3980,7 +3989,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>45</v>
       </c>
@@ -4012,7 +4021,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>62</v>
       </c>
@@ -4044,7 +4053,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>65</v>
       </c>
@@ -4076,7 +4085,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>72</v>
       </c>
@@ -4108,7 +4117,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>86</v>
       </c>

</xml_diff>